<commit_message>
aqui vamos de nuevo
</commit_message>
<xml_diff>
--- a/web/upload/FormatoCargaCliente.xlsx
+++ b/web/upload/FormatoCargaCliente.xlsx
@@ -1,30 +1,65 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoelvys\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1719E8-32E1-417F-A2CD-4FBE0A878FAD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Usuario de Windows</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar codigo según tipo de identificacion</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+04 - Ruc
+05 - Cedula
+06 - Pasaporte
+07 - Consumidor Final
+08 - Identificacion del Exterior
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
   <si>
     <t>Nombre</t>
   </si>
@@ -44,50 +79,332 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Yoelvys Martinez</t>
-  </si>
-  <si>
     <t>04</t>
   </si>
   <si>
-    <t>0978845222</t>
-  </si>
-  <si>
-    <t>Mariana de Jesus</t>
-  </si>
-  <si>
-    <t>0997739485</t>
-  </si>
-  <si>
-    <t>y@gmail.com</t>
-  </si>
-  <si>
-    <t>Joel Alejandro</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>1311692139001</t>
-  </si>
-  <si>
-    <t>1311692139</t>
-  </si>
-  <si>
-    <t>Karen Bermeo</t>
-  </si>
-  <si>
-    <t>Quito El inca</t>
-  </si>
-  <si>
-    <t>k@gmail.com</t>
+    <t>ALTA PRODUCTIVIDAD Y SERVICIOS ALPROS S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUDITAR DEL ECUADOR </t>
+  </si>
+  <si>
+    <t>CLIMBING TOUR</t>
+  </si>
+  <si>
+    <t>CONSORCIO KLAERE ISAMEL WORLD</t>
+  </si>
+  <si>
+    <t>CRIDEGCOM</t>
+  </si>
+  <si>
+    <t>DATILMEDIA S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAVID HIDALGO EUSSE </t>
+  </si>
+  <si>
+    <t>DICOMVISEK CIA LTDA</t>
+  </si>
+  <si>
+    <t>ECUADORIANPIPE CIA. LTDA.</t>
+  </si>
+  <si>
+    <t>ENGIPETROL S.A</t>
+  </si>
+  <si>
+    <t>HOSTELERIA SAN AGUSTIN DE CALLO HOSACSA S.A.</t>
+  </si>
+  <si>
+    <t>INSTITUTO DE ESTUDIOS ECUATORIANOS</t>
+  </si>
+  <si>
+    <t>OSORIO VARGAS JUAN FAUSTINO</t>
+  </si>
+  <si>
+    <t>RODRIGUEZ VILLEGAS DANIEL JESUS</t>
+  </si>
+  <si>
+    <t>SANCHEZ CORREA MIRIAM MARGARITA</t>
+  </si>
+  <si>
+    <t>SANDRA PALACIOS LANGUAGE SERVICES CIA.LTDA.</t>
+  </si>
+  <si>
+    <t>SOLMOCONTADORES</t>
+  </si>
+  <si>
+    <t>SONDA DEL ECUADOR ECUASONDA S.A.</t>
+  </si>
+  <si>
+    <t>SWISSMED PHARMACEUTICAL</t>
+  </si>
+  <si>
+    <t>TECNISUPPORT CIA. LTDA.</t>
+  </si>
+  <si>
+    <t>TECNOMEGA C.A.</t>
+  </si>
+  <si>
+    <t>WORLD POS SOLUTIONS CIA. LTDA</t>
+  </si>
+  <si>
+    <t>JUAN LEON MERA Y WILSON</t>
+  </si>
+  <si>
+    <t>AV. AMAZONAZ N21-221 Y RAMON ROCA</t>
+  </si>
+  <si>
+    <t>ELOY VELASQUEZ MZ #32 - SOLAR #30 GUAYAQUIL</t>
+  </si>
+  <si>
+    <t>AV.6 DE DICIEMBRE N26-66 Y SAN IGNACIO</t>
+  </si>
+  <si>
+    <t>TORRES DEL NORTE, TORRE A PISO 3 OFICINA 308</t>
+  </si>
+  <si>
+    <t>AZCUNAGA 282 Y AV BRASIL</t>
+  </si>
+  <si>
+    <t>DUCHICELA 530 Y 9 DE AGOSTO - CALDERON</t>
+  </si>
+  <si>
+    <t>JOAQUIN PINTO E4-286 Y AMAZONAS</t>
+  </si>
+  <si>
+    <t>LASSO - COTOPAXI, A 77 KM. AL SUR DE QUITO POR LA CARRETERA PANAMERICANA SUR. 5 KM.</t>
+  </si>
+  <si>
+    <t>AV.10 AGOSTO N25-39 Y COLON</t>
+  </si>
+  <si>
+    <t>AV. DE LOS SHYRIS N33-134 Y AV. REPUBLICA DEL SALVADOR</t>
+  </si>
+  <si>
+    <t>ANTONIO ROMAN OE8-89 Y IGNACIO ASIN</t>
+  </si>
+  <si>
+    <t>CONOCOTO</t>
+  </si>
+  <si>
+    <t>JUAN PABLO SANZ N35-26 Y JUAN GONZALES</t>
+  </si>
+  <si>
+    <t>ALARCON FALCONI E18A 15PB</t>
+  </si>
+  <si>
+    <t>1792381339001</t>
+  </si>
+  <si>
+    <t>1708979420001</t>
+  </si>
+  <si>
+    <t>1792603005001</t>
+  </si>
+  <si>
+    <t>1791329732001</t>
+  </si>
+  <si>
+    <t>1791712927001</t>
+  </si>
+  <si>
+    <t>1715516124001</t>
+  </si>
+  <si>
+    <t>1791728963001</t>
+  </si>
+  <si>
+    <t>1791955072001</t>
+  </si>
+  <si>
+    <t>1712716974001</t>
+  </si>
+  <si>
+    <t>1792130824001</t>
+  </si>
+  <si>
+    <t>1792440467001</t>
+  </si>
+  <si>
+    <t>1790726681001</t>
+  </si>
+  <si>
+    <t>1792644313001</t>
+  </si>
+  <si>
+    <t>1792590574001</t>
+  </si>
+  <si>
+    <t>1791433025001</t>
+  </si>
+  <si>
+    <t>1792057302001</t>
+  </si>
+  <si>
+    <t>1791254791001</t>
+  </si>
+  <si>
+    <t>1792477522001</t>
+  </si>
+  <si>
+    <t>1792510899001</t>
+  </si>
+  <si>
+    <t>1792418445001</t>
+  </si>
+  <si>
+    <t>1704900834001</t>
+  </si>
+  <si>
+    <t>02 2906157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02256 3036 </t>
+  </si>
+  <si>
+    <t>cponce@apsalpros.com</t>
+  </si>
+  <si>
+    <t>aromasyespecias@gmail.com</t>
+  </si>
+  <si>
+    <t>operaciones@auditar.ec</t>
+  </si>
+  <si>
+    <t>info@climbingtour.com</t>
+  </si>
+  <si>
+    <t>compras@estruturasklaere.com</t>
+  </si>
+  <si>
+    <t>informacion.uio@cridegcom.com</t>
+  </si>
+  <si>
+    <t>clientes@datilmedia.com</t>
+  </si>
+  <si>
+    <t>davidhidalgoe@gmail.com</t>
+  </si>
+  <si>
+    <t>compras@dicomvisek.com</t>
+  </si>
+  <si>
+    <t>pvasquez@ecuadorianpipe.net</t>
+  </si>
+  <si>
+    <t>info@electtel.com</t>
+  </si>
+  <si>
+    <t>elsa.eggestol@engipetrol.com</t>
+  </si>
+  <si>
+    <t>contabilidad@incahacienda.com</t>
+  </si>
+  <si>
+    <t>ocaru2012@gmail.com</t>
+  </si>
+  <si>
+    <t>asistente@itq.edu.ec</t>
+  </si>
+  <si>
+    <t>lumasa08@gmail.com</t>
+  </si>
+  <si>
+    <t>juanfosorio6@hotmail.com</t>
+  </si>
+  <si>
+    <t>ventas@favolahosting.com</t>
+  </si>
+  <si>
+    <t>conmaco2005@gmail.com</t>
+  </si>
+  <si>
+    <t>splanguageservicesquito@gmail.com</t>
+  </si>
+  <si>
+    <t>info@solmocontadores.com</t>
+  </si>
+  <si>
+    <t>comprobantes.electronicos.ecu@sonda.com</t>
+  </si>
+  <si>
+    <t>echiriboga@swissmedpharmaceutical.com</t>
+  </si>
+  <si>
+    <t>contabilidad@tecnisupport.com.ec</t>
+  </si>
+  <si>
+    <t>jbenavides@tecnomega.com</t>
+  </si>
+  <si>
+    <t>administrativo@wposs.com</t>
+  </si>
+  <si>
+    <t>San Ignacio E9-182(123) y Av. 6 de Diciembre. Of. 2</t>
+  </si>
+  <si>
+    <t>Guayaqanes Mz98 Villa 4</t>
+  </si>
+  <si>
+    <t>Floresta 2 Mz. 170 villa 14. Segundo piso.</t>
+  </si>
+  <si>
+    <t>Av Shyris N36-166 Y nnuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Av.Shirys N36-188 y Naciones unidas </t>
+  </si>
+  <si>
+    <t>Av. Colon E2-56 Y Av. Nueve De Octubre Quito - Ecuador</t>
+  </si>
+  <si>
+    <t>El Mercurio 236 y La Razon. (Tras el Quicentro Norte)</t>
+  </si>
+  <si>
+    <t>LA kennedy,Cap. Ramon Borja E6211 y Bejamin Franklin</t>
+  </si>
+  <si>
+    <t>AV. CRISToBAL COLON E4-105 ENTRE 9 DE OCTUBRE Y AMAZONAS</t>
+  </si>
+  <si>
+    <t>JOSe ENRIQUEZ N64-365</t>
+  </si>
+  <si>
+    <t>Twin Towers, Av Republica de El Salvador,  N35-104, Quito</t>
+  </si>
+  <si>
+    <t>INSTITUTO TECNOLOGICO QUITO</t>
+  </si>
+  <si>
+    <t>LUIS MALDONADO HOLGUIN</t>
+  </si>
+  <si>
+    <t>EDWIN ESTRELLA PEREZ</t>
+  </si>
+  <si>
+    <t>Arboleda ArEvalo carlos Alberto</t>
+  </si>
+  <si>
+    <t>0920707882001</t>
+  </si>
+  <si>
+    <t>0907913628001</t>
+  </si>
+  <si>
+    <t>0992942401001</t>
+  </si>
+  <si>
+    <t>0992712554001</t>
+  </si>
+  <si>
+    <t>0601708779001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,12 +413,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,17 +443,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,21 +731,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="63.7109375" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="59.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -448,58 +770,527 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="2">
+        <v>22527991</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="2">
+        <v>28811059</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2234350</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3814960</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2">
+        <v>42113516</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2556655</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="2">
+        <v>46029400</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="2">
+        <v>23320039</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="2">
+        <v>22024120</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="2">
+        <v>23453150</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="2">
+        <v>6014358</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="2">
+        <v>22248688</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2904098</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="2">
+        <v>225126340</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="2">
+        <v>99999999</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3824692</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="2">
+        <v>99999999</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2433276</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="2">
+        <v>22268559</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="2">
+        <v>99999999</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3731570</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="2">
+        <v>22926038</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2254459</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="2">
+        <v>22503183</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>